<commit_message>
first automation flow added...
</commit_message>
<xml_diff>
--- a/TestData/bulkEditOptions.xlsx
+++ b/TestData/bulkEditOptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E11844-0281-40E9-9A44-EDD559190E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DFE59F-A94E-475E-9175-00D2DEEC2359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3336" yWindow="1896" windowWidth="18756" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2748" yWindow="2256" windowWidth="18756" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Goal</t>
   </si>
@@ -84,7 +84,16 @@
     <t>TNG (Yes / No)</t>
   </si>
   <si>
-    <t>OCI Trial</t>
+    <t>Allow FS Deletion (Yes/No)</t>
+  </si>
+  <si>
+    <t>Event Script</t>
+  </si>
+  <si>
+    <t>Event Script Args</t>
+  </si>
+  <si>
+    <t>First Flow</t>
   </si>
 </sst>
 </file>
@@ -411,7 +420,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -419,7 +428,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
@@ -437,9 +446,12 @@
     <col min="16" max="16" width="26.21875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -494,10 +506,19 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>

</xml_diff>